<commit_message>
fix: estandarizar nombre archivo Excel exportado a formato N-XXX-26 [Modulo] V04
</commit_message>
<xml_diff>
--- a/app/templates/Template_Verificacion.xlsx
+++ b/app/templates/Template_Verificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\crmnew\api-geofal-crm\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C35724-0714-42F7-BFDD-586EACC99938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FE8053-403C-4698-9B9C-C33A81264433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A76715E4-29FC-4532-A462-AEFC175FF6CC}"/>
   </bookViews>
@@ -1517,60 +1517,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -1593,44 +1539,209 @@
     <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1644,149 +1755,38 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2542,8 +2542,8 @@
   </sheetPr>
   <dimension ref="A1:V44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2573,111 +2573,111 @@
       <c r="A1" s="65"/>
       <c r="B1" s="66"/>
       <c r="C1" s="67"/>
-      <c r="D1" s="140" t="s">
+      <c r="D1" s="123" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="140"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
-      <c r="J1" s="140"/>
-      <c r="K1" s="140"/>
-      <c r="L1" s="140"/>
-      <c r="M1" s="140"/>
-      <c r="N1" s="140"/>
-      <c r="O1" s="140"/>
-      <c r="P1" s="140"/>
-      <c r="Q1" s="140"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="123"/>
+      <c r="L1" s="123"/>
+      <c r="M1" s="123"/>
+      <c r="N1" s="123"/>
+      <c r="O1" s="123"/>
+      <c r="P1" s="123"/>
+      <c r="Q1" s="123"/>
       <c r="R1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="137" t="s">
+      <c r="S1" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="137"/>
-      <c r="U1" s="137"/>
+      <c r="T1" s="120"/>
+      <c r="U1" s="120"/>
     </row>
     <row r="2" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="68"/>
       <c r="B2" s="4"/>
       <c r="C2" s="69"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="140"/>
-      <c r="F2" s="140"/>
-      <c r="G2" s="140"/>
-      <c r="H2" s="140"/>
-      <c r="I2" s="140"/>
-      <c r="J2" s="140"/>
-      <c r="K2" s="140"/>
-      <c r="L2" s="140"/>
-      <c r="M2" s="140"/>
-      <c r="N2" s="140"/>
-      <c r="O2" s="140"/>
-      <c r="P2" s="140"/>
-      <c r="Q2" s="140"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="123"/>
+      <c r="Q2" s="123"/>
       <c r="R2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="138">
+      <c r="S2" s="121">
         <v>3</v>
       </c>
-      <c r="T2" s="138"/>
-      <c r="U2" s="138"/>
+      <c r="T2" s="121"/>
+      <c r="U2" s="121"/>
     </row>
     <row r="3" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="68"/>
       <c r="B3" s="4"/>
       <c r="C3" s="69"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="140"/>
-      <c r="F3" s="140"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="140"/>
-      <c r="I3" s="140"/>
-      <c r="J3" s="140"/>
-      <c r="K3" s="140"/>
-      <c r="L3" s="140"/>
-      <c r="M3" s="140"/>
-      <c r="N3" s="140"/>
-      <c r="O3" s="140"/>
-      <c r="P3" s="140"/>
-      <c r="Q3" s="140"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="123"/>
+      <c r="N3" s="123"/>
+      <c r="O3" s="123"/>
+      <c r="P3" s="123"/>
+      <c r="Q3" s="123"/>
       <c r="R3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="S3" s="139">
-        <v>45726</v>
-      </c>
-      <c r="T3" s="139"/>
-      <c r="U3" s="139"/>
+      <c r="S3" s="122">
+        <v>46070</v>
+      </c>
+      <c r="T3" s="122"/>
+      <c r="U3" s="122"/>
     </row>
     <row r="4" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="70"/>
       <c r="B4" s="71"/>
       <c r="C4" s="72"/>
-      <c r="D4" s="140"/>
-      <c r="E4" s="140"/>
-      <c r="F4" s="140"/>
-      <c r="G4" s="140"/>
-      <c r="H4" s="140"/>
-      <c r="I4" s="140"/>
-      <c r="J4" s="140"/>
-      <c r="K4" s="140"/>
-      <c r="L4" s="140"/>
-      <c r="M4" s="140"/>
-      <c r="N4" s="140"/>
-      <c r="O4" s="140"/>
-      <c r="P4" s="140"/>
-      <c r="Q4" s="140"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="123"/>
+      <c r="M4" s="123"/>
+      <c r="N4" s="123"/>
+      <c r="O4" s="123"/>
+      <c r="P4" s="123"/>
+      <c r="Q4" s="123"/>
       <c r="R4" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="137" t="s">
+      <c r="S4" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="T4" s="137"/>
-      <c r="U4" s="137"/>
+      <c r="T4" s="120"/>
+      <c r="U4" s="120"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
@@ -2703,20 +2703,20 @@
       <c r="B6" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="135" t="s">
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="135"/>
-      <c r="L6" s="135"/>
-      <c r="M6" s="134"/>
-      <c r="N6" s="134"/>
+      <c r="K6" s="118"/>
+      <c r="L6" s="118"/>
+      <c r="M6" s="117"/>
+      <c r="N6" s="117"/>
       <c r="P6" s="76" t="s">
         <v>53</v>
       </c>
@@ -2727,68 +2727,68 @@
       <c r="A7" s="23"/>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="125"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
-      <c r="J7" s="126"/>
-      <c r="K7" s="126"/>
-      <c r="L7" s="126"/>
+      <c r="D7" s="124"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
+      <c r="J7" s="125"/>
+      <c r="K7" s="125"/>
+      <c r="L7" s="125"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="128" t="s">
+      <c r="A8" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="128" t="s">
+      <c r="B8" s="127" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="130" t="s">
+      <c r="C8" s="129" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="118" t="s">
+      <c r="D8" s="134" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="118"/>
-      <c r="F8" s="118"/>
-      <c r="G8" s="118"/>
-      <c r="H8" s="119" t="s">
+      <c r="E8" s="134"/>
+      <c r="F8" s="134"/>
+      <c r="G8" s="134"/>
+      <c r="H8" s="135" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="120"/>
-      <c r="J8" s="120"/>
-      <c r="K8" s="120"/>
-      <c r="L8" s="121"/>
-      <c r="M8" s="118" t="s">
+      <c r="I8" s="136"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="136"/>
+      <c r="L8" s="137"/>
+      <c r="M8" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="N8" s="118"/>
-      <c r="O8" s="118"/>
-      <c r="P8" s="132" t="s">
+      <c r="N8" s="134"/>
+      <c r="O8" s="134"/>
+      <c r="P8" s="131" t="s">
         <v>85</v>
       </c>
-      <c r="Q8" s="132" t="s">
+      <c r="Q8" s="131" t="s">
         <v>87</v>
       </c>
-      <c r="R8" s="122" t="s">
+      <c r="R8" s="138" t="s">
         <v>89</v>
       </c>
-      <c r="S8" s="123"/>
-      <c r="T8" s="124"/>
-      <c r="U8" s="117" t="s">
+      <c r="S8" s="139"/>
+      <c r="T8" s="140"/>
+      <c r="U8" s="133" t="s">
         <v>90</v>
       </c>
-      <c r="V8" s="117"/>
+      <c r="V8" s="133"/>
     </row>
     <row r="9" spans="1:22" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="129"/>
-      <c r="B9" s="129"/>
-      <c r="C9" s="131"/>
+      <c r="A9" s="128"/>
+      <c r="B9" s="128"/>
+      <c r="C9" s="130"/>
       <c r="D9" s="87" t="s">
         <v>36</v>
       </c>
@@ -2825,8 +2825,8 @@
       <c r="O9" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="P9" s="133"/>
-      <c r="Q9" s="133"/>
+      <c r="P9" s="132"/>
+      <c r="Q9" s="132"/>
       <c r="R9" s="87" t="s">
         <v>56</v>
       </c>
@@ -2836,8 +2836,8 @@
       <c r="T9" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="U9" s="117"/>
-      <c r="V9" s="117"/>
+      <c r="U9" s="133"/>
+      <c r="V9" s="133"/>
     </row>
     <row r="10" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
@@ -3109,25 +3109,25 @@
       <c r="R20" s="2"/>
     </row>
     <row r="21" spans="1:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="127" t="s">
+      <c r="A21" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="127"/>
-      <c r="C21" s="127"/>
-      <c r="D21" s="127"/>
-      <c r="E21" s="127"/>
-      <c r="F21" s="127"/>
-      <c r="G21" s="127"/>
-      <c r="H21" s="127"/>
-      <c r="I21" s="127"/>
-      <c r="J21" s="127"/>
-      <c r="K21" s="127"/>
-      <c r="L21" s="127"/>
-      <c r="M21" s="127"/>
-      <c r="N21" s="127"/>
-      <c r="O21" s="127"/>
-      <c r="P21" s="127"/>
-      <c r="Q21" s="127"/>
+      <c r="B21" s="126"/>
+      <c r="C21" s="126"/>
+      <c r="D21" s="126"/>
+      <c r="E21" s="126"/>
+      <c r="F21" s="126"/>
+      <c r="G21" s="126"/>
+      <c r="H21" s="126"/>
+      <c r="I21" s="126"/>
+      <c r="J21" s="126"/>
+      <c r="K21" s="126"/>
+      <c r="L21" s="126"/>
+      <c r="M21" s="126"/>
+      <c r="N21" s="126"/>
+      <c r="O21" s="126"/>
+      <c r="P21" s="126"/>
+      <c r="Q21" s="126"/>
       <c r="R21" s="2"/>
     </row>
     <row r="22" spans="1:22" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3496,6 +3496,19 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="U8:V9"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="A21:Q21"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="C6:I6"/>
@@ -3504,19 +3517,6 @@
     <mergeCell ref="S3:U3"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="D1:Q4"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="A21:Q21"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="U8:V9"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="H8:L8"/>
-    <mergeCell ref="R8:T8"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0" footer="0"/>
@@ -3680,110 +3680,110 @@
       <c r="A1" s="65"/>
       <c r="B1" s="66"/>
       <c r="C1" s="67"/>
-      <c r="D1" s="143" t="s">
+      <c r="D1" s="193" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="144"/>
-      <c r="L1" s="144"/>
-      <c r="M1" s="144"/>
-      <c r="N1" s="144"/>
-      <c r="O1" s="144"/>
-      <c r="P1" s="144"/>
-      <c r="Q1" s="145"/>
+      <c r="E1" s="194"/>
+      <c r="F1" s="194"/>
+      <c r="G1" s="194"/>
+      <c r="H1" s="194"/>
+      <c r="I1" s="194"/>
+      <c r="J1" s="194"/>
+      <c r="K1" s="194"/>
+      <c r="L1" s="194"/>
+      <c r="M1" s="194"/>
+      <c r="N1" s="194"/>
+      <c r="O1" s="194"/>
+      <c r="P1" s="194"/>
+      <c r="Q1" s="195"/>
       <c r="R1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="152" t="s">
+      <c r="S1" s="202" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="153"/>
+      <c r="T1" s="203"/>
       <c r="U1" s="1"/>
     </row>
     <row r="2" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="68"/>
       <c r="B2" s="4"/>
       <c r="C2" s="69"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
-      <c r="H2" s="147"/>
-      <c r="I2" s="147"/>
-      <c r="J2" s="147"/>
-      <c r="K2" s="147"/>
-      <c r="L2" s="147"/>
-      <c r="M2" s="147"/>
-      <c r="N2" s="147"/>
-      <c r="O2" s="147"/>
-      <c r="P2" s="147"/>
-      <c r="Q2" s="148"/>
+      <c r="D2" s="196"/>
+      <c r="E2" s="197"/>
+      <c r="F2" s="197"/>
+      <c r="G2" s="197"/>
+      <c r="H2" s="197"/>
+      <c r="I2" s="197"/>
+      <c r="J2" s="197"/>
+      <c r="K2" s="197"/>
+      <c r="L2" s="197"/>
+      <c r="M2" s="197"/>
+      <c r="N2" s="197"/>
+      <c r="O2" s="197"/>
+      <c r="P2" s="197"/>
+      <c r="Q2" s="198"/>
       <c r="R2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="152">
+      <c r="S2" s="202">
         <v>1</v>
       </c>
-      <c r="T2" s="153"/>
+      <c r="T2" s="203"/>
       <c r="U2" s="1"/>
     </row>
     <row r="3" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="68"/>
       <c r="B3" s="4"/>
       <c r="C3" s="69"/>
-      <c r="D3" s="146"/>
-      <c r="E3" s="147"/>
-      <c r="F3" s="147"/>
-      <c r="G3" s="147"/>
-      <c r="H3" s="147"/>
-      <c r="I3" s="147"/>
-      <c r="J3" s="147"/>
-      <c r="K3" s="147"/>
-      <c r="L3" s="147"/>
-      <c r="M3" s="147"/>
-      <c r="N3" s="147"/>
-      <c r="O3" s="147"/>
-      <c r="P3" s="147"/>
-      <c r="Q3" s="148"/>
+      <c r="D3" s="196"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="197"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="197"/>
+      <c r="I3" s="197"/>
+      <c r="J3" s="197"/>
+      <c r="K3" s="197"/>
+      <c r="L3" s="197"/>
+      <c r="M3" s="197"/>
+      <c r="N3" s="197"/>
+      <c r="O3" s="197"/>
+      <c r="P3" s="197"/>
+      <c r="Q3" s="198"/>
       <c r="R3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="S3" s="152">
+      <c r="S3" s="202">
         <v>45232</v>
       </c>
-      <c r="T3" s="153"/>
+      <c r="T3" s="203"/>
       <c r="U3" s="1"/>
     </row>
     <row r="4" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="70"/>
       <c r="B4" s="71"/>
       <c r="C4" s="72"/>
-      <c r="D4" s="149"/>
-      <c r="E4" s="150"/>
-      <c r="F4" s="150"/>
-      <c r="G4" s="150"/>
-      <c r="H4" s="150"/>
-      <c r="I4" s="150"/>
-      <c r="J4" s="150"/>
-      <c r="K4" s="150"/>
-      <c r="L4" s="150"/>
-      <c r="M4" s="150"/>
-      <c r="N4" s="150"/>
-      <c r="O4" s="150"/>
-      <c r="P4" s="150"/>
-      <c r="Q4" s="151"/>
+      <c r="D4" s="199"/>
+      <c r="E4" s="200"/>
+      <c r="F4" s="200"/>
+      <c r="G4" s="200"/>
+      <c r="H4" s="200"/>
+      <c r="I4" s="200"/>
+      <c r="J4" s="200"/>
+      <c r="K4" s="200"/>
+      <c r="L4" s="200"/>
+      <c r="M4" s="200"/>
+      <c r="N4" s="200"/>
+      <c r="O4" s="200"/>
+      <c r="P4" s="200"/>
+      <c r="Q4" s="201"/>
       <c r="R4" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="152" t="s">
+      <c r="S4" s="202" t="s">
         <v>4</v>
       </c>
-      <c r="T4" s="153"/>
+      <c r="T4" s="203"/>
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -3816,16 +3816,16 @@
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
       <c r="D6" s="27"/>
-      <c r="E6" s="154"/>
-      <c r="F6" s="154"/>
+      <c r="E6" s="189"/>
+      <c r="F6" s="189"/>
       <c r="G6" s="28"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="155" t="s">
+      <c r="J6" s="190" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="155"/>
-      <c r="L6" s="155"/>
+      <c r="K6" s="190"/>
+      <c r="L6" s="190"/>
       <c r="M6" s="33"/>
       <c r="N6" s="52"/>
       <c r="O6" s="33"/>
@@ -3843,11 +3843,11 @@
       <c r="D7" s="18"/>
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="156"/>
-      <c r="H7" s="156"/>
-      <c r="I7" s="156"/>
-      <c r="J7" s="156"/>
-      <c r="K7" s="156"/>
+      <c r="G7" s="191"/>
+      <c r="H7" s="191"/>
+      <c r="I7" s="191"/>
+      <c r="J7" s="191"/>
+      <c r="K7" s="191"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -3861,10 +3861,10 @@
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
       <c r="D8" s="29"/>
-      <c r="E8" s="157"/>
-      <c r="F8" s="157"/>
-      <c r="G8" s="157"/>
-      <c r="H8" s="157"/>
+      <c r="E8" s="192"/>
+      <c r="F8" s="192"/>
+      <c r="G8" s="192"/>
+      <c r="H8" s="192"/>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
       <c r="K8" s="34"/>
@@ -3884,10 +3884,10 @@
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="29"/>
-      <c r="E9" s="157"/>
-      <c r="F9" s="157"/>
-      <c r="G9" s="157"/>
-      <c r="H9" s="157"/>
+      <c r="E9" s="192"/>
+      <c r="F9" s="192"/>
+      <c r="G9" s="192"/>
+      <c r="H9" s="192"/>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
       <c r="K9" s="34"/>
@@ -3903,19 +3903,19 @@
       <c r="A10" s="23"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
-      <c r="D10" s="125" t="s">
+      <c r="D10" s="124" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="125"/>
-      <c r="F10" s="125"/>
-      <c r="G10" s="125"/>
-      <c r="H10" s="126" t="s">
+      <c r="E10" s="124"/>
+      <c r="F10" s="124"/>
+      <c r="G10" s="124"/>
+      <c r="H10" s="125" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="126"/>
-      <c r="J10" s="126"/>
-      <c r="K10" s="126"/>
-      <c r="L10" s="126"/>
+      <c r="I10" s="125"/>
+      <c r="J10" s="125"/>
+      <c r="K10" s="125"/>
+      <c r="L10" s="125"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
@@ -3923,116 +3923,116 @@
       <c r="U10" s="1"/>
     </row>
     <row r="11" spans="1:21" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="158" t="s">
+      <c r="A11" s="181" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="159" t="s">
+      <c r="B11" s="182" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="160" t="s">
+      <c r="C11" s="175" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="163" t="s">
+      <c r="D11" s="184" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="164"/>
-      <c r="F11" s="164"/>
-      <c r="G11" s="165"/>
-      <c r="H11" s="166" t="s">
+      <c r="E11" s="185"/>
+      <c r="F11" s="185"/>
+      <c r="G11" s="186"/>
+      <c r="H11" s="187" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="167"/>
-      <c r="J11" s="167"/>
-      <c r="K11" s="167"/>
-      <c r="L11" s="167"/>
-      <c r="M11" s="168" t="s">
+      <c r="I11" s="188"/>
+      <c r="J11" s="188"/>
+      <c r="K11" s="188"/>
+      <c r="L11" s="188"/>
+      <c r="M11" s="157" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="169"/>
-      <c r="O11" s="169"/>
-      <c r="P11" s="169"/>
-      <c r="Q11" s="169"/>
-      <c r="R11" s="170" t="s">
+      <c r="N11" s="158"/>
+      <c r="O11" s="158"/>
+      <c r="P11" s="158"/>
+      <c r="Q11" s="158"/>
+      <c r="R11" s="159" t="s">
         <v>34</v>
       </c>
-      <c r="S11" s="171"/>
-      <c r="T11" s="176" t="s">
+      <c r="S11" s="160"/>
+      <c r="T11" s="165" t="s">
         <v>33</v>
       </c>
       <c r="U11" s="1"/>
     </row>
     <row r="12" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="158"/>
-      <c r="B12" s="159"/>
-      <c r="C12" s="161"/>
-      <c r="D12" s="178" t="s">
+      <c r="A12" s="181"/>
+      <c r="B12" s="182"/>
+      <c r="C12" s="183"/>
+      <c r="D12" s="167" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="179"/>
-      <c r="F12" s="179"/>
-      <c r="G12" s="180"/>
-      <c r="H12" s="178" t="s">
+      <c r="E12" s="168"/>
+      <c r="F12" s="168"/>
+      <c r="G12" s="169"/>
+      <c r="H12" s="167" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="179"/>
-      <c r="J12" s="179"/>
-      <c r="K12" s="179"/>
-      <c r="L12" s="180"/>
-      <c r="M12" s="178" t="s">
+      <c r="I12" s="168"/>
+      <c r="J12" s="168"/>
+      <c r="K12" s="168"/>
+      <c r="L12" s="169"/>
+      <c r="M12" s="167" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="179"/>
-      <c r="O12" s="179"/>
-      <c r="P12" s="179"/>
-      <c r="Q12" s="179"/>
-      <c r="R12" s="172"/>
-      <c r="S12" s="173"/>
-      <c r="T12" s="177"/>
+      <c r="N12" s="168"/>
+      <c r="O12" s="168"/>
+      <c r="P12" s="168"/>
+      <c r="Q12" s="168"/>
+      <c r="R12" s="161"/>
+      <c r="S12" s="162"/>
+      <c r="T12" s="166"/>
     </row>
     <row r="13" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="158"/>
-      <c r="B13" s="159"/>
-      <c r="C13" s="161"/>
-      <c r="D13" s="181" t="s">
+      <c r="A13" s="181"/>
+      <c r="B13" s="182"/>
+      <c r="C13" s="183"/>
+      <c r="D13" s="170" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="117" t="s">
+      <c r="E13" s="133" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="182" t="s">
+      <c r="F13" s="171" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="183"/>
-      <c r="H13" s="184" t="s">
+      <c r="G13" s="172"/>
+      <c r="H13" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="185"/>
-      <c r="J13" s="185"/>
-      <c r="K13" s="185"/>
-      <c r="L13" s="160" t="s">
+      <c r="I13" s="174"/>
+      <c r="J13" s="174"/>
+      <c r="K13" s="174"/>
+      <c r="L13" s="175" t="s">
         <v>41</v>
       </c>
-      <c r="M13" s="186" t="s">
+      <c r="M13" s="177" t="s">
         <v>24</v>
       </c>
-      <c r="N13" s="187"/>
-      <c r="O13" s="188" t="s">
+      <c r="N13" s="178"/>
+      <c r="O13" s="179" t="s">
         <v>25</v>
       </c>
-      <c r="P13" s="188"/>
+      <c r="P13" s="179"/>
       <c r="Q13" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="R13" s="172"/>
-      <c r="S13" s="173"/>
-      <c r="T13" s="177"/>
+      <c r="R13" s="161"/>
+      <c r="S13" s="162"/>
+      <c r="T13" s="166"/>
     </row>
     <row r="14" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="158"/>
-      <c r="B14" s="159"/>
-      <c r="C14" s="162"/>
-      <c r="D14" s="181"/>
-      <c r="E14" s="117"/>
+      <c r="A14" s="181"/>
+      <c r="B14" s="182"/>
+      <c r="C14" s="176"/>
+      <c r="D14" s="170"/>
+      <c r="E14" s="133"/>
       <c r="F14" s="62" t="s">
         <v>28</v>
       </c>
@@ -4051,21 +4051,21 @@
       <c r="K14" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="L14" s="162"/>
-      <c r="M14" s="189" t="s">
+      <c r="L14" s="176"/>
+      <c r="M14" s="180" t="s">
         <v>23</v>
       </c>
-      <c r="N14" s="120"/>
-      <c r="O14" s="119" t="s">
+      <c r="N14" s="136"/>
+      <c r="O14" s="135" t="s">
         <v>23</v>
       </c>
-      <c r="P14" s="121"/>
+      <c r="P14" s="137"/>
       <c r="Q14" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="R14" s="174"/>
-      <c r="S14" s="175"/>
-      <c r="T14" s="177"/>
+      <c r="R14" s="163"/>
+      <c r="S14" s="164"/>
+      <c r="T14" s="166"/>
     </row>
     <row r="15" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
@@ -4100,13 +4100,13 @@
       <c r="L15" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="M15" s="190"/>
-      <c r="N15" s="191"/>
-      <c r="O15" s="190"/>
-      <c r="P15" s="191"/>
+      <c r="M15" s="155"/>
+      <c r="N15" s="156"/>
+      <c r="O15" s="155"/>
+      <c r="P15" s="156"/>
       <c r="Q15" s="58"/>
-      <c r="R15" s="192"/>
-      <c r="S15" s="193"/>
+      <c r="R15" s="149"/>
+      <c r="S15" s="150"/>
       <c r="T15" s="64"/>
     </row>
     <row r="16" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4127,21 +4127,21 @@
       <c r="J16" s="46"/>
       <c r="K16" s="47"/>
       <c r="L16" s="42"/>
-      <c r="M16" s="194" t="s">
+      <c r="M16" s="145" t="s">
         <v>44</v>
       </c>
-      <c r="N16" s="195"/>
-      <c r="O16" s="196" t="s">
+      <c r="N16" s="146"/>
+      <c r="O16" s="147" t="s">
         <v>44</v>
       </c>
-      <c r="P16" s="197"/>
+      <c r="P16" s="148"/>
       <c r="Q16" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="R16" s="192" t="s">
+      <c r="R16" s="149" t="s">
         <v>15</v>
       </c>
-      <c r="S16" s="193"/>
+      <c r="S16" s="150"/>
       <c r="T16" s="64" t="s">
         <v>15</v>
       </c>
@@ -4161,21 +4161,21 @@
       <c r="J17" s="46"/>
       <c r="K17" s="47"/>
       <c r="L17" s="42"/>
-      <c r="M17" s="194" t="s">
+      <c r="M17" s="145" t="s">
         <v>45</v>
       </c>
-      <c r="N17" s="195"/>
-      <c r="O17" s="196" t="s">
+      <c r="N17" s="146"/>
+      <c r="O17" s="147" t="s">
         <v>46</v>
       </c>
-      <c r="P17" s="197"/>
+      <c r="P17" s="148"/>
       <c r="Q17" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="R17" s="198" t="s">
+      <c r="R17" s="151" t="s">
         <v>48</v>
       </c>
-      <c r="S17" s="199"/>
+      <c r="S17" s="152"/>
       <c r="T17" s="64" t="s">
         <v>46</v>
       </c>
@@ -4195,21 +4195,21 @@
       <c r="J18" s="46"/>
       <c r="K18" s="47"/>
       <c r="L18" s="42"/>
-      <c r="M18" s="194" t="s">
+      <c r="M18" s="145" t="s">
         <v>45</v>
       </c>
-      <c r="N18" s="195"/>
-      <c r="O18" s="196" t="s">
+      <c r="N18" s="146"/>
+      <c r="O18" s="147" t="s">
         <v>46</v>
       </c>
-      <c r="P18" s="197"/>
+      <c r="P18" s="148"/>
       <c r="Q18" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="R18" s="200" t="s">
+      <c r="R18" s="153" t="s">
         <v>47</v>
       </c>
-      <c r="S18" s="201"/>
+      <c r="S18" s="154"/>
       <c r="T18" s="64" t="s">
         <v>46</v>
       </c>
@@ -4229,13 +4229,13 @@
       <c r="J19" s="46"/>
       <c r="K19" s="47"/>
       <c r="L19" s="42"/>
-      <c r="M19" s="194"/>
-      <c r="N19" s="195"/>
-      <c r="O19" s="196"/>
-      <c r="P19" s="197"/>
+      <c r="M19" s="145"/>
+      <c r="N19" s="146"/>
+      <c r="O19" s="147"/>
+      <c r="P19" s="148"/>
       <c r="Q19" s="58"/>
-      <c r="R19" s="192"/>
-      <c r="S19" s="193"/>
+      <c r="R19" s="149"/>
+      <c r="S19" s="150"/>
       <c r="T19" s="64"/>
     </row>
     <row r="20" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4253,13 +4253,13 @@
       <c r="J20" s="46"/>
       <c r="K20" s="47"/>
       <c r="L20" s="42"/>
-      <c r="M20" s="194"/>
-      <c r="N20" s="195"/>
-      <c r="O20" s="196"/>
-      <c r="P20" s="197"/>
+      <c r="M20" s="145"/>
+      <c r="N20" s="146"/>
+      <c r="O20" s="147"/>
+      <c r="P20" s="148"/>
       <c r="Q20" s="58"/>
-      <c r="R20" s="192"/>
-      <c r="S20" s="193"/>
+      <c r="R20" s="149"/>
+      <c r="S20" s="150"/>
       <c r="T20" s="64"/>
     </row>
     <row r="21" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4277,13 +4277,13 @@
       <c r="J21" s="46"/>
       <c r="K21" s="47"/>
       <c r="L21" s="42"/>
-      <c r="M21" s="194"/>
-      <c r="N21" s="195"/>
-      <c r="O21" s="196"/>
-      <c r="P21" s="197"/>
+      <c r="M21" s="145"/>
+      <c r="N21" s="146"/>
+      <c r="O21" s="147"/>
+      <c r="P21" s="148"/>
       <c r="Q21" s="58"/>
-      <c r="R21" s="192"/>
-      <c r="S21" s="193"/>
+      <c r="R21" s="149"/>
+      <c r="S21" s="150"/>
       <c r="T21" s="64"/>
     </row>
     <row r="22" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4301,13 +4301,13 @@
       <c r="J22" s="46"/>
       <c r="K22" s="47"/>
       <c r="L22" s="42"/>
-      <c r="M22" s="194"/>
-      <c r="N22" s="195"/>
-      <c r="O22" s="196"/>
-      <c r="P22" s="197"/>
+      <c r="M22" s="145"/>
+      <c r="N22" s="146"/>
+      <c r="O22" s="147"/>
+      <c r="P22" s="148"/>
       <c r="Q22" s="58"/>
-      <c r="R22" s="192"/>
-      <c r="S22" s="193"/>
+      <c r="R22" s="149"/>
+      <c r="S22" s="150"/>
       <c r="T22" s="64"/>
     </row>
     <row r="23" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4325,13 +4325,13 @@
       <c r="J23" s="46"/>
       <c r="K23" s="47"/>
       <c r="L23" s="42"/>
-      <c r="M23" s="194"/>
-      <c r="N23" s="195"/>
-      <c r="O23" s="196"/>
-      <c r="P23" s="197"/>
+      <c r="M23" s="145"/>
+      <c r="N23" s="146"/>
+      <c r="O23" s="147"/>
+      <c r="P23" s="148"/>
       <c r="Q23" s="58"/>
-      <c r="R23" s="192"/>
-      <c r="S23" s="193"/>
+      <c r="R23" s="149"/>
+      <c r="S23" s="150"/>
       <c r="T23" s="64"/>
     </row>
     <row r="24" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4349,13 +4349,13 @@
       <c r="J24" s="46"/>
       <c r="K24" s="47"/>
       <c r="L24" s="42"/>
-      <c r="M24" s="194"/>
-      <c r="N24" s="195"/>
-      <c r="O24" s="196"/>
-      <c r="P24" s="197"/>
+      <c r="M24" s="145"/>
+      <c r="N24" s="146"/>
+      <c r="O24" s="147"/>
+      <c r="P24" s="148"/>
       <c r="Q24" s="58"/>
-      <c r="R24" s="192"/>
-      <c r="S24" s="193"/>
+      <c r="R24" s="149"/>
+      <c r="S24" s="150"/>
       <c r="T24" s="64"/>
     </row>
     <row r="25" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4373,13 +4373,13 @@
       <c r="J25" s="46"/>
       <c r="K25" s="47"/>
       <c r="L25" s="42"/>
-      <c r="M25" s="194"/>
-      <c r="N25" s="195"/>
-      <c r="O25" s="196"/>
-      <c r="P25" s="197"/>
+      <c r="M25" s="145"/>
+      <c r="N25" s="146"/>
+      <c r="O25" s="147"/>
+      <c r="P25" s="148"/>
       <c r="Q25" s="58"/>
-      <c r="R25" s="192"/>
-      <c r="S25" s="193"/>
+      <c r="R25" s="149"/>
+      <c r="S25" s="150"/>
       <c r="T25" s="64"/>
     </row>
     <row r="26" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4397,13 +4397,13 @@
       <c r="J26" s="46"/>
       <c r="K26" s="47"/>
       <c r="L26" s="42"/>
-      <c r="M26" s="194"/>
-      <c r="N26" s="195"/>
-      <c r="O26" s="196"/>
-      <c r="P26" s="197"/>
+      <c r="M26" s="145"/>
+      <c r="N26" s="146"/>
+      <c r="O26" s="147"/>
+      <c r="P26" s="148"/>
       <c r="Q26" s="58"/>
-      <c r="R26" s="192"/>
-      <c r="S26" s="193"/>
+      <c r="R26" s="149"/>
+      <c r="S26" s="150"/>
       <c r="T26" s="64"/>
     </row>
     <row r="27" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4421,13 +4421,13 @@
       <c r="J27" s="46"/>
       <c r="K27" s="47"/>
       <c r="L27" s="42"/>
-      <c r="M27" s="194"/>
-      <c r="N27" s="195"/>
-      <c r="O27" s="196"/>
-      <c r="P27" s="197"/>
+      <c r="M27" s="145"/>
+      <c r="N27" s="146"/>
+      <c r="O27" s="147"/>
+      <c r="P27" s="148"/>
       <c r="Q27" s="58"/>
-      <c r="R27" s="192"/>
-      <c r="S27" s="193"/>
+      <c r="R27" s="149"/>
+      <c r="S27" s="150"/>
       <c r="T27" s="64"/>
     </row>
     <row r="28" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4445,13 +4445,13 @@
       <c r="J28" s="46"/>
       <c r="K28" s="47"/>
       <c r="L28" s="42"/>
-      <c r="M28" s="194"/>
-      <c r="N28" s="195"/>
-      <c r="O28" s="196"/>
-      <c r="P28" s="197"/>
+      <c r="M28" s="145"/>
+      <c r="N28" s="146"/>
+      <c r="O28" s="147"/>
+      <c r="P28" s="148"/>
       <c r="Q28" s="59"/>
-      <c r="R28" s="192"/>
-      <c r="S28" s="193"/>
+      <c r="R28" s="149"/>
+      <c r="S28" s="150"/>
       <c r="T28" s="64"/>
     </row>
     <row r="29" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4535,12 +4535,12 @@
       <c r="U32" s="2"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="202" t="s">
+      <c r="A33" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="202"/>
-      <c r="C33" s="202"/>
-      <c r="D33" s="202"/>
+      <c r="B33" s="143"/>
+      <c r="C33" s="143"/>
+      <c r="D33" s="143"/>
       <c r="E33" s="35"/>
       <c r="F33" s="35"/>
       <c r="G33" s="35"/>
@@ -4560,12 +4560,12 @@
       <c r="U33" s="2"/>
     </row>
     <row r="34" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="203" t="s">
+      <c r="A34" s="144" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="203"/>
-      <c r="C34" s="203"/>
-      <c r="D34" s="203"/>
+      <c r="B34" s="144"/>
+      <c r="C34" s="144"/>
+      <c r="D34" s="144"/>
       <c r="E34" s="36"/>
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
@@ -4608,28 +4608,28 @@
       <c r="U35" s="2"/>
     </row>
     <row r="36" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="127" t="s">
+      <c r="A36" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="127"/>
-      <c r="C36" s="127"/>
-      <c r="D36" s="127"/>
-      <c r="E36" s="127"/>
-      <c r="F36" s="127"/>
-      <c r="G36" s="127"/>
-      <c r="H36" s="127"/>
-      <c r="I36" s="127"/>
-      <c r="J36" s="127"/>
-      <c r="K36" s="127"/>
-      <c r="L36" s="127"/>
-      <c r="M36" s="127"/>
-      <c r="N36" s="127"/>
-      <c r="O36" s="127"/>
-      <c r="P36" s="127"/>
-      <c r="Q36" s="127"/>
-      <c r="R36" s="127"/>
-      <c r="S36" s="127"/>
-      <c r="T36" s="127"/>
+      <c r="B36" s="126"/>
+      <c r="C36" s="126"/>
+      <c r="D36" s="126"/>
+      <c r="E36" s="126"/>
+      <c r="F36" s="126"/>
+      <c r="G36" s="126"/>
+      <c r="H36" s="126"/>
+      <c r="I36" s="126"/>
+      <c r="J36" s="126"/>
+      <c r="K36" s="126"/>
+      <c r="L36" s="126"/>
+      <c r="M36" s="126"/>
+      <c r="N36" s="126"/>
+      <c r="O36" s="126"/>
+      <c r="P36" s="126"/>
+      <c r="Q36" s="126"/>
+      <c r="R36" s="126"/>
+      <c r="S36" s="126"/>
+      <c r="T36" s="126"/>
       <c r="U36" s="2"/>
     </row>
     <row r="37" spans="1:21" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5049,51 +5049,23 @@
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A36:T36"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="R27:S27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="R28:S28"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="D1:Q4"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="H10:L10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="H11:L11"/>
     <mergeCell ref="M11:Q11"/>
     <mergeCell ref="R11:S14"/>
     <mergeCell ref="T11:T14"/>
@@ -5109,23 +5081,51 @@
     <mergeCell ref="O13:P13"/>
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="O14:P14"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="D1:Q4"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A36:T36"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="R28:S28"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="0.19685039370078741" bottom="0.15748031496062992" header="0" footer="0.31496062992125984"/>

</xml_diff>